<commit_message>
fix logic import student
</commit_message>
<xml_diff>
--- a/storage/app/templates/template-import-siswa.xlsx
+++ b/storage/app/templates/template-import-siswa.xlsx
@@ -8,64 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\php\laravel-school\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A613F9-C960-4D87-B68C-F74D50CF5A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6748B6B4-08A3-461E-A9E4-68738037061C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21825" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4140" yWindow="8790" windowWidth="21825" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template Siswa" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>nama_lengkap</t>
+    <t>Nama Lengkap*</t>
   </si>
   <si>
-    <t>nama_orang_tua</t>
+    <t>Orang Tua/Wali*</t>
   </si>
   <si>
-    <t>kelas</t>
+    <t>Kelas</t>
   </si>
   <si>
-    <t>nis</t>
+    <t>NIS</t>
   </si>
   <si>
-    <t>tahun_masuk</t>
+    <t>Tahun Masuk*</t>
   </si>
   <si>
-    <t>jenis_kelamin</t>
+    <t>Jenis Kelamin*</t>
   </si>
   <si>
-    <t>status</t>
+    <t>Agama</t>
   </si>
   <si>
-    <t>agama</t>
+    <t>Tempat Lahir</t>
   </si>
   <si>
-    <t>tempat_lahir</t>
+    <t>Tanggal Lahir</t>
   </si>
   <si>
-    <t>tanggal_lahir</t>
-  </si>
-  <si>
-    <t>alamat</t>
+    <t>Alamat</t>
   </si>
 </sst>
 </file>
@@ -73,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -111,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,20 +118,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -615,15 +636,13 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11">
       <c r="J2" s="2"/>

</xml_diff>